<commit_message>
Actualización Base de datos y bitácora
Se actualizo los diagramas junto con la base de datos y restricciones,
se anexaron las funciones para la aplicación.
</commit_message>
<xml_diff>
--- a/7_ADMON_PROYECTO/BITACORAS/PARCIAL_1/BITACORA_1P.xlsx
+++ b/7_ADMON_PROYECTO/BITACORAS/PARCIAL_1/BITACORA_1P.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cely\Documents\Proyecto 6\Bitácora\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cely\Documents\ADMON_PROYECTO\BITACORAS\PARCIAL_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="70">
   <si>
     <t>Grupo:</t>
   </si>
@@ -334,12 +334,25 @@
   <si>
     <t>Elaboración del diseño de las interfaces de la aplicación</t>
   </si>
+  <si>
+    <t xml:space="preserve">Diagrama Entidad-Relación
+Modelo lógico y fisíco de la base de datos       Diccionario de base de datos
+Restricciones de base de datos         Minuta    </t>
+  </si>
+  <si>
+    <t>Especificación de requerimientos
+Minuta</t>
+  </si>
+  <si>
+    <t>Diseño de las ventanas
+Minuta</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -409,6 +422,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FF00B0F0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -728,10 +749,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -910,8 +932,17 @@
     <xf numFmtId="0" fontId="4" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1704,7 +1735,7 @@
   <dimension ref="B2:K109"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1805,7 +1836,7 @@
       <c r="F9" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="G9" s="12" t="s">
+      <c r="G9" s="72" t="s">
         <v>51</v>
       </c>
       <c r="H9" s="11" t="s">
@@ -1829,8 +1860,8 @@
       <c r="F10" s="34" t="s">
         <v>62</v>
       </c>
-      <c r="G10" s="12" t="s">
-        <v>51</v>
+      <c r="G10" s="73" t="s">
+        <v>68</v>
       </c>
       <c r="H10" s="11" t="s">
         <v>44</v>
@@ -1853,8 +1884,8 @@
       <c r="F11" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="G11" s="12" t="s">
-        <v>51</v>
+      <c r="G11" s="73" t="s">
+        <v>67</v>
       </c>
       <c r="H11" s="11" t="s">
         <v>47</v>
@@ -1877,8 +1908,8 @@
       <c r="F12" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="G12" s="12" t="s">
-        <v>51</v>
+      <c r="G12" s="73" t="s">
+        <v>69</v>
       </c>
       <c r="H12" s="11" t="s">
         <v>46</v>
@@ -2864,9 +2895,15 @@
       <formula2>15</formula2>
     </dataValidation>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="G9" r:id="rId1"/>
+    <hyperlink ref="G10" r:id="rId2" display="SEMANA_2"/>
+    <hyperlink ref="G11" r:id="rId3" display="SEMANA_3"/>
+    <hyperlink ref="G12" r:id="rId4" display="SEMANA_4"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="300" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageSetup orientation="portrait" verticalDpi="300" r:id="rId5"/>
+  <drawing r:id="rId6"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
@@ -2898,8 +2935,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:U40"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageBreakPreview" topLeftCell="A3" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="W17" sqref="W17"/>
+    <sheetView showGridLines="0" view="pageBreakPreview" topLeftCell="A6" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="L28" sqref="L28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3355,7 +3392,7 @@
       <c r="H20" s="4"/>
       <c r="I20" s="32"/>
       <c r="J20" s="32"/>
-      <c r="K20" s="4"/>
+      <c r="K20" s="21"/>
       <c r="L20" s="4"/>
       <c r="M20" s="4"/>
       <c r="N20" s="4"/>

</xml_diff>